<commit_message>
Csa pratiques 1 & 2 archi
</commit_message>
<xml_diff>
--- a/Cas pratique/cas_pratique_archi_1/PPN_MAT_PVDS_light.xlsx
+++ b/Cas pratique/cas_pratique_archi_1/PPN_MAT_PVDS_light.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alban.peyrat\Documents\_Code\OpenRefine_Formation\OpenRefine-Formation\Cas pratique\cas_pratique_archi_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E633DE-59CD-47E7-A5E1-887A167B8A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6547A3D8-B7EA-484B-83CE-B05D4E53A027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19420" yWindow="13590" windowWidth="19360" windowHeight="10360" xr2:uid="{5E215C95-45ED-4CA5-9152-C84A57801431}"/>
+    <workbookView xWindow="-19450" yWindow="13560" windowWidth="19420" windowHeight="10420" xr2:uid="{5E215C95-45ED-4CA5-9152-C84A57801431}"/>
   </bookViews>
   <sheets>
     <sheet name="ED_iln428_ppn" sheetId="1" r:id="rId1"/>
@@ -20,54 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>00419747X</t>
   </si>
   <si>
-    <t>003723801</t>
-  </si>
-  <si>
-    <t>023557222</t>
-  </si>
-  <si>
-    <t>011958510</t>
-  </si>
-  <si>
-    <t>023557249</t>
-  </si>
-  <si>
-    <t>124635660</t>
-  </si>
-  <si>
     <t>06096216X</t>
-  </si>
-  <si>
-    <t>003730948</t>
-  </si>
-  <si>
-    <t>026240580</t>
-  </si>
-  <si>
-    <t>052182657</t>
-  </si>
-  <si>
-    <t>288470788</t>
-  </si>
-  <si>
-    <t>088605094</t>
-  </si>
-  <si>
-    <t>224310739</t>
-  </si>
-  <si>
-    <t>039222454</t>
-  </si>
-  <si>
-    <t>250010194</t>
-  </si>
-  <si>
-    <t>278389236</t>
   </si>
 </sst>
 </file>
@@ -551,9 +509,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,7 +891,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,78 +902,78 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>3723801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>23557222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>11958510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>23557249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>124635660</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+      <c r="A8" s="1">
+        <v>3730948</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" s="1">
+        <v>26240580</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+      <c r="A10" s="1">
+        <v>52182657</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+      <c r="A11" s="1">
+        <v>288470788</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+      <c r="A12" s="1">
+        <v>88605094</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+      <c r="A13" s="1">
+        <v>224310739</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+      <c r="A14" s="1">
+        <v>39222454</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
+      <c r="A15" s="1">
+        <v>250010194</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+      <c r="A16" s="1">
+        <v>278389236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>